<commit_message>
fixed prisma.fi, tokmanni EAN control logic
</commit_message>
<xml_diff>
--- a/kilpailijahintoja.xlsx
+++ b/kilpailijahintoja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slambe\Desktop\UNI\ohjelmointi\Python\SOK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D3146C-93B7-45C1-AD00-8C0C3A281329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E08E8A5-815C-42AD-9C01-2A6348DF22BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$3:$J$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$3:$J$26</definedName>
     <definedName name="ID" localSheetId="0" hidden="1">"49e52ab4-2dac-4e78-a94d-74337646439d"</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentManualCount="12"/>
@@ -533,11 +533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J27"/>
+  <dimension ref="A3:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +587,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>3606480504662</v>
+        <v>3606480504679</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -595,13 +595,13 @@
       <c r="E4" s="8"/>
       <c r="F4" s="9"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="9"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>3606480504679</v>
+        <v>3606481825353</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -609,13 +609,13 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="7"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>3606481825353</v>
+        <v>3606481825377</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>3606481825377</v>
+        <v>3606481825384</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -639,11 +639,11 @@
       <c r="G7" s="7"/>
       <c r="H7" s="9"/>
       <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>3606481825384</v>
+        <v>3606481825445</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -653,11 +653,11 @@
       <c r="G8" s="7"/>
       <c r="H8" s="9"/>
       <c r="I8" s="7"/>
-      <c r="J8" s="9"/>
+      <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>3606481825445</v>
+        <v>3606481825452</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -671,21 +671,21 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>3606481825452</v>
+        <v>6418677309526</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="9"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="9"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>6418677309526</v>
+        <v>6418677309533</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -699,7 +699,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>6418677309533</v>
+        <v>6418677310003</v>
       </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -713,7 +713,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>6418677310003</v>
+        <v>6418677310010</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>6418677310010</v>
+        <v>6418677310539</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -741,7 +741,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>6418677310539</v>
+        <v>6418677310560</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -755,7 +755,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>6418677310560</v>
+        <v>6418677310607</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -769,7 +769,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>6418677310607</v>
+        <v>6418677310690</v>
       </c>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -783,7 +783,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>6418677310690</v>
+        <v>6418677330599</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -797,7 +797,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <v>6418677330599</v>
+        <v>6418677333002</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -805,41 +805,41 @@
       <c r="E19" s="6"/>
       <c r="F19" s="9"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="9"/>
       <c r="I19" s="7"/>
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <v>6418677333002</v>
+        <v>6418677333040</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="6"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="9"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <v>6418677333040</v>
+        <v>6418677333255</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="9"/>
       <c r="I21" s="7"/>
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <v>6418677333255</v>
+        <v>6418677333262</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -853,7 +853,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <v>6418677333262</v>
+        <v>6418677333316</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -867,21 +867,21 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <v>6418677333316</v>
+        <v>6418677334924</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="6"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="9"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <v>6418677334924</v>
+        <v>6418677334948</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -889,13 +889,13 @@
       <c r="E25" s="6"/>
       <c r="F25" s="9"/>
       <c r="G25" s="10"/>
-      <c r="H25" s="7"/>
+      <c r="H25" s="9"/>
       <c r="I25" s="7"/>
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>6418677334948</v>
+        <v>6438199001944</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -905,26 +905,12 @@
       <c r="G26" s="10"/>
       <c r="H26" s="9"/>
       <c r="I26" s="7"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
-        <v>6438199001944</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
+      <c r="J26" s="7"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:J27" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J27">
-      <sortCondition ref="A3:A27"/>
+  <autoFilter ref="A3:J26" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J26">
+      <sortCondition ref="A3:A26"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added debugging file separately
</commit_message>
<xml_diff>
--- a/kilpailijahintoja.xlsx
+++ b/kilpailijahintoja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slambe\Desktop\UNI\ohjelmointi\Python\SOK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E08E8A5-815C-42AD-9C01-2A6348DF22BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC645CC3-E17B-4572-B065-C54EA89568AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>EAN</t>
   </si>
@@ -54,6 +54,24 @@
   </si>
   <si>
     <t>Tokmanni linkki</t>
+  </si>
+  <si>
+    <t>IDO</t>
+  </si>
+  <si>
+    <t>Ido Glow Z6700100001 painonappi täydellinen krom</t>
+  </si>
+  <si>
+    <t>Wc-varaosa IDO Z6700100001 2-toiminen painike kromi Glow</t>
+  </si>
+  <si>
+    <t>Gustavsberg Nautic 9GN01161 huuhtelupainike duo kromi matala</t>
+  </si>
+  <si>
+    <t>Gustavsberg</t>
+  </si>
+  <si>
+    <t>Wc-varaosa Gustavsberg Nautic HF painonappi Duo matala kromi</t>
   </si>
 </sst>
 </file>
@@ -108,7 +126,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +161,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor rgb="FF90EE90"/>
       </patternFill>
     </fill>
   </fills>
@@ -212,10 +236,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -537,7 +561,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,325 +611,198 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <v>3606480504679</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="9"/>
+        <v>7391515432435</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>21.9</v>
+      </c>
+      <c r="E4" s="6">
+        <v>21.95</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <v>3606481825353</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+        <v>4051202546182</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>31.9</v>
+      </c>
+      <c r="E5" s="6">
+        <v>41.95</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <v>3606481825377</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+        <v>6416129362310</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <v>3606481825384</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="9"/>
+        <v>6416129362556</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="7"/>
+      <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>3606481825445</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+        <v>6416129362525</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>3606481825452</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+        <v>7391515121926</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>6418677309526</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+        <v>7391515117301</v>
+      </c>
+      <c r="D10" s="9"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="9"/>
+      <c r="F10" s="7"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>6418677309533</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+        <v>7391515121353</v>
+      </c>
       <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="9"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>6418677310003</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+        <v>7391515121346</v>
+      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="9"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>6418677310010</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+        <v>6418677333255</v>
+      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="6"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="9"/>
+      <c r="F13" s="7"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>6418677310539</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+        <v>6418677333262</v>
+      </c>
       <c r="E14" s="6"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="9"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>6418677310560</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+        <v>6418677333316</v>
+      </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="9"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="9"/>
+      <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>6418677310607</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+        <v>6418677334924</v>
+      </c>
       <c r="E16" s="6"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="9"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>6418677310690</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+        <v>6418677334948</v>
+      </c>
       <c r="E17" s="6"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="9"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="10"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>6418677330599</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+        <v>6438199001944</v>
+      </c>
       <c r="E18" s="6"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="9"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>6418677333002</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="9"/>
+      <c r="H19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>6418677333040</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="9"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>6418677333255</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="9"/>
+      <c r="H21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>6418677333262</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="9"/>
+      <c r="H22" s="7"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>6418677333316</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="9"/>
+      <c r="H23" s="7"/>
+      <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>6418677334924</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>6418677334948</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="9"/>
+      <c r="H25" s="7"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
-        <v>6438199001944</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:J26" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -913,6 +810,12 @@
       <sortCondition ref="A3:A26"/>
     </sortState>
   </autoFilter>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>